<commit_message>
2024-04-25 Post CRUD ~ing
2024-04-25 Post CRUD ~ing
</commit_message>
<xml_diff>
--- a/강현욱TIL.xlsx
+++ b/강현욱TIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kang\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7510CC79-CE7D-4D6F-B8FE-F0A6FB5A8AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC0361C-47CD-48E2-A0B7-965372B8BFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6AE18CFE-AA7A-4E33-95E8-8EB9E27EF076}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
   <si>
     <t>날짜</t>
   </si>
@@ -6542,10 +6542,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>JSTL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>나는 오전에 CRUD 중 Delete 부분을 구현해봄</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -6906,12 +6902,663 @@
 </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>나는 오전에 게시판 CRUD구현에 대해서 공부함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 오후에 게시판 CRUD구현에 대해서 공부함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;%@ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFC792EA"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">page </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFFFCB6B"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>contentType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFEEFFFF"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC3E88D"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>text/html;charset=UTF-8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFEEFFFF"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFFFCB6B"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>language</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFEEFFFF"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC3E88D"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>java</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFEEFFFF"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC3E88D"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">%&gt;
+&lt;%@ page import="kr.co.bit.BoardDAO" %&gt;
+&lt;%@ page import="kr.co.bit.BoardBean" %&gt;
+&lt;%@ page contentType="text/html;charset=UTF-8" language="java" %&gt;
+&lt;html&gt;
+&lt;head&gt;
+    &lt;title&gt;Title&lt;/title&gt;
+&lt;/head&gt;
+&lt;body&gt;
+&lt;%
+    // 게시글 상세보기를 하기 위해 BoardList에서 전달받은 num값을 가지고 와서
+    int num = Integer.parseInt(request.getParameter("num").trim()); // trim은 공백제거
+    BoardDAO bdao = new BoardDAO();
+    BoardBean bean = bdao.oneBoard(num); // 한 게시물 상세보기를 한다
+%&gt;
+&lt;h2&gt;Post of One&lt;/h2&gt;
+&lt;table width="600" border="1"&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="120" align="center"&gt;No.&lt;/td&gt;
+        &lt;td width="120" align="center"&gt;&lt;%=bean.getNum()%&gt;
+        &lt;/td&gt;
+        &lt;td width="120" align="center"&gt;Count&lt;/td&gt;
+        &lt;td width="120" align="center"&gt;&lt;%=bean.getReadcount()%&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="120" align="center"&gt;Writer&lt;/td&gt;
+        &lt;td width="120" align="center"&gt;&lt;%=bean.getWriter()%&gt;
+        &lt;/td&gt;
+        &lt;td width="120" align="center"&gt;Date&lt;/td&gt;
+        &lt;td width="120" align="center"&gt;&lt;%=bean.getReg_date()%&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="120" align="center"&gt;Email&lt;/td&gt;
+        &lt;td width="120" align="center" colspan="3"&gt;&lt;%=bean.getEmail()%&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="120" align="center"&gt;Subject&lt;/td&gt;
+        &lt;td width="120" align="center" colspan="3"&gt;&lt;%=bean.getSubject()%&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="120" align="center"&gt;Content&lt;/td&gt;
+        &lt;td width="120" align="center" colspan="3"&gt;&lt;%=bean.getContent()%&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="200" align="center" colspan="4"&gt;
+            &lt;input type="button" value="comment"
+                   onclick="location.href='ReWriteForm.jsp?num=&lt;%=bean.getNum() %&gt;&amp;ref=&lt;%=bean.getRef() %&gt;&amp;re_step=&lt;%=bean.getRe_step() %&gt;&amp;re_level=&lt;%=bean.getRe_level() %&gt;'"&gt;
+            &lt;input type="button" value="Modify" onclick="location.href='UpdateForm.jsp?num=&lt;%=bean.getNum()%&gt;'"&gt; &lt;!-- UpdateForm -&gt; 글번호 가지고 --&gt;
+            &lt;input type="button" value="Delete" onclick="location.href='DeleteForm.jsp?num=&lt;%=bean.getNum()%&gt;'"&gt; &lt;!-- DeleteForm -&gt; 글번호 --&gt;
+            &lt;input type="button" value="List" onclick="location.href='BoardList.jsp'"&gt; &lt;!-- BoardList  --&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+&lt;/table&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+&lt;%@ page import="kr.co.bit.BoardDAO" %&gt;
+&lt;%@ page import="kr.co.bit.BoardBean" %&gt;
+&lt;%@ page import="java.util.Vector" %&gt;
+&lt;%@ page contentType="text/html;charset=UTF-8" language="java" %&gt;
+&lt;html&gt;
+&lt;body&gt;
+&lt;h2&gt;All Post&lt;/h2&gt;
+    &lt;%
+        int pageSize=10; // 페이지당 보여지는 게시글 수
+        String pageNum=request.getParameter("pageNum"); // 페이지 번호
+        if(pageNum==null){
+            pageNum="1";
+        }
+    int count = 0; // 전체 글 갯수 알아내기 위해 설정
+    int number = 0;
+    BoardDAO bdao = new BoardDAO();
+    count = bdao.getAllCount(); // 전체 게시글 개수 읽어온다
+    int currentPage = Integer.parseInt(pageNum); // 현재 페이지 번호
+    int startRow=(currentPage-1)*pageSize+1;
+            //         1-1*10+1
+    int endRow=currentPage * pageSize; // 1*10
+        Vector&lt;BoardBean&gt; vec = bdao.allBoard(startRow, endRow);
+        number = count - (currentPage -1) * pageSize;
+%&gt;
+&lt;table width="800" border="1"&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="50" allign="center"&gt;No.&lt;/td&gt;
+        &lt;td width="420" allign="center"&gt;Subject&lt;/td&gt;
+        &lt;td width="100" allign="center"&gt;Writer&lt;/td&gt;
+        &lt;td width="150" allign="center"&gt;Date&lt;/td&gt;
+        &lt;td width="80" allign="center"&gt;Count&lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;%
+        for (int i = 0; i &lt; vec.size(); i++) {
+            BoardBean bean = vec.get(i);
+    %&gt;
+    &lt;tr height="40"&gt;
+        &lt;td width="50" align="center"&gt;&lt;%=number--%&gt;
+        &lt;/td&gt;
+        &lt;td width="420" align="center"&gt;
+            &lt;a href="BoardIn.jsp?num=&lt;%=bean.getNum() %&gt;" style="text-decoration: none"&gt; &lt;!-- 글번호 --&gt;
+                &lt;%=bean.getSubject() %&gt;&lt;!-- 브라우저에 출력되는 제목이름 --&gt;&lt;/a&gt;&lt;/td&gt;
+        &lt;td width="100" align="center"&gt;&lt;%=bean.getWriter() %&gt;
+        &lt;/td&gt;
+        &lt;td width="150" align="center"&gt;&lt;%=bean.getReg_date() %&gt;
+        &lt;/td&gt;
+        &lt;td width="80" align="center"&gt;&lt;%=bean.getReadcount() %&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;%
+        }
+    %&gt;
+    &lt;tr height="40"&gt;
+        &lt;td colspan="5" align="center"&gt;
+            &lt;input type="button" value="Write" onclick="location.href='BoardForm.jsp'"&gt;
+        &lt;/td&gt;
+    &lt;/tr&gt;
+&lt;/table&gt;
+    &lt;%
+    if(count &gt; 0){    //  127 / 10  + 1  =  13
+        int pageCount = count/pageSize + (count % pageSize == 0  ? 0 : 1); // 페이지 수 계산
+        // 총 페이지 수
+        int startPage=1;
+        if(currentPage % 10 !=0){ // currentPage가 11인 경우
+            startPage = (int)(currentPage / 10) * 10 + 1; // 한 줄 안에 있는 페이지 개수
+        }
+        else { // currentPage가 10인 경우
+            startPage =((int)(currentPage / 10)-1) * 10 + 1; // 한 �� 안에 있는
+        }
+        int pageBlock=10;
+        int endPage = startPage + pageBlock - 1;
+        if(endPage &gt; pageCount)
+            endPage = pageCount;
+    //이전이라는 하이퍼링크 만들건지 생각
+    if(startPage&gt;10){
+    %&gt;
+    &lt;a href="BoardList.jsp?pageNum=&lt;%=startPage-10 %&gt;"&gt;[Before]&lt;/a&gt;
+    &lt;%
+    }
+    for(int i=startPage;i&lt;=endPage;i++){
+    %&gt;
+    &lt;a href="BoardList.jsp?pageNum=&lt;%=i %&gt;"&gt;[&lt;%=i %&gt;]&lt;/a&gt;
+    &lt;%
+    }
+    if(endPage &lt; pageCount){
+    %&gt;
+    &lt;a href="BoardList.jsp?pageNum=&lt;%=startPage+10 %&gt;"&gt;[After]&lt;/a&gt;
+    &lt;%
+    }
+    }
+%&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+&lt;%@ page import="kr.co.bit.BoardDAO" %&gt;
+&lt;%@ page contentType="text/html;charset=UTF-8" language="java" %&gt;
+&lt;html&gt;
+&lt;body&gt;
+&lt;%
+    request.setCharacterEncoding("UTF-8");
+    response.setContentType("text/html; charset=UTF-8");
+%&gt;
+&lt;jsp:useBean id="boardbean" class="kr.co.bit.BoardBean"&gt;
+    &lt;jsp:setProperty name="boardbean" property="*"/&gt;
+&lt;/jsp:useBean&gt;
+&lt;%
+    BoardDAO bdao = new BoardDAO();
+    bdao.insertBoard(boardbean);
+    response.sendRedirect("BoardList.jsp"); // 글쓰기 한 후 바로 글 쓴 목록을 보기 위해서
+%&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+&lt;%@ page import="java.sql.Connection" %&gt;
+&lt;%@ page import="bit.dao.MemberDAO" %&gt;
+&lt;%@ page contentType="text/html;charset=UTF-8" language="java" %&gt;
+&lt;html&gt;
+&lt;head&gt;
+    &lt;title&gt;Title&lt;/title&gt;
+&lt;/head&gt;
+&lt;body&gt;
+&lt;%
+    MemberDAO dao = MemberDAO.getInstance();
+    Connection conn =dao.getConnection();
+    out.print("연동성공");
+%&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+&lt;%@ page import="kr.co.bit.BoardDAO" %&gt;
+&lt;%@ page import="kr.co.bit.BoardBean" %&gt;
+&lt;%@ page contentType="text/html;charset=UTF-8" language="java" %&gt;
+&lt;html&gt;
+&lt;head&gt;
+    &lt;title&gt;Title&lt;/title&gt;
+&lt;/head&gt;
+&lt;body&gt;
+&lt;h2&gt;Modify a Post&lt;/h2&gt;
+&lt;%
+    int num = Integer.parseInt(request.getParameter("num"));
+    BoardDAO dao = new BoardDAO();
+    BoardBean bean = dao.oneUpdateBoard(num);
+%&gt;
+&lt;form action="UpdateProc.jsp" method="post"&gt;
+    &lt;table width="600" border="1"&gt;
+        &lt;tr height="40"&gt;
+            &lt;td align="center" width="150"&gt;Writer&lt;/td&gt;
+            &lt;td align="center" width="150"&gt;&lt;%=bean.getWriter() %&gt;
+            &lt;/td&gt;
+            &lt;td align="center" width="150"&gt;Registed Date&lt;/td&gt;
+            &lt;td align="center" width="150"&gt;&lt;%=bean.getReg_date() %&gt;
+            &lt;/td&gt;
+        &lt;/tr&gt;
+        &lt;tr height="40"&gt;
+            &lt;td align="center" width="150"&gt;Subject&lt;/td&gt;
+            &lt;td width="150" colspan="3"&gt;&amp;nbsp;&lt;input type="text" name="subject" value="&lt;%=bean.getSubject()%&gt;"&gt;&lt;/td&gt;
+        &lt;/tr&gt;
+        &lt;tr height="40"&gt;
+            &lt;td align="center" width="150"&gt;Password&lt;/td&gt;
+            &lt;td width="150" colspan="3"&gt;&amp;nbsp;
+                &lt;input type="password" name="password" value="&lt;%=bean.getPassword()%&gt;"&gt;&lt;/td&gt;
+        &lt;/tr&gt;
+        &lt;tr height="40"&gt;
+            &lt;td align="center" width="150"&gt;Content&lt;/td&gt;
+            &lt;td width="150" colspan="3"&gt;&amp;nbsp;
+                &lt;textarea rows="10" cols="50" name="content"&gt;&lt;%=bean.getContent()%&gt;&lt;/textarea&gt;
+            &lt;/td&gt;
+        &lt;/tr&gt;
+        &lt;tr height="40"&gt;
+            &lt;td width="150" colspan="4"&gt;&amp;nbsp;
+                &lt;input type="hidden" name="num" value="&lt;%=bean.getNum()%&gt;"&gt;
+                &lt;input type="submit" value="Modify"&gt;&amp;nbsp;
+                &lt;input type="button" onclick="location.href='BoardList.jsp'" value="All PostList"&gt;
+            &lt;/td&gt;
+        &lt;/tr&gt;
+    &lt;/table&gt;
+&lt;/form&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+&lt;%@ page import="kr.co.bit.BoardDAO" %&gt;
+&lt;%@ page contentType="text/html;charset=UTF-8" language="java" %&gt;
+&lt;html&gt;
+&lt;head&gt;
+    &lt;title&gt;Title&lt;/title&gt;
+&lt;/head&gt;
+&lt;body&gt;
+    &lt;%
+        request.setCharacterEncoding("UTF-8");
+    %&gt;
+    &lt;jsp:useBean id="boardbean" class="kr.co.bit.BoardBean"&gt;
+        &lt;jsp:setProperty name="boardbean" property="*"/&gt;
+    &lt;/jsp:useBean&gt;
+    &lt;%
+        BoardDAO bdao=new BoardDAO();
+        String pass=bdao.getPass(boardbean.getNum()); //hidden 으로 넘긴값 받기
+       //DB에 있는값             폼에 입력한 값
+        if(pass.equals(boardbean.getPassword())){
+            bdao.updateBoard(boardbean);
+            response.sendRedirect("BoardList.jsp");
+        }
+        else{
+            %&gt;
+    &lt;script type="text/javascript"&gt;
+        alert("Incorrect Password, Retry again.");
+        history.go(-1);
+    &lt;/script&gt;
+    &lt;%
+        }
+    %&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+package kr.co.bit;
+import javax.naming.Context;
+import javax.naming.InitialContext;
+import javax.sql.DataSource;
+import java.sql.Connection;
+import java.sql.PreparedStatement;
+import java.sql.ResultSet;
+import java.util.Vector;
+public class BoardDAO {
+    Connection con;
+    PreparedStatement pstmt;
+    ResultSet rs;
+    public void getCon() { // DB연결 작업 DBCP
+        try {
+            Context init = new InitialContext();
+            //JNDI(Java Naming and Directory Interface)를 사용하여 초기 컨텍스트를 설정하는 것
+            DataSource ds = (DataSource) init.lookup("java:comp/env/jdbc/pool"); // Server.xml에 추가한 dbcp환경설정 불러오기
+            con = ds.getConnection();
+        } catch (Exception e) {
+            e.printStackTrace();
+        }
+    }
+    public void insertBoard(BoardBean bean) {
+        getCon();
+        int ref = 0;
+        int re_step = 1;
+        int re_level = 1;
+        try {
+            String rsql = "select max(ref) from board";
+            pstmt = con.prepareStatement(rsql);
+            rs = pstmt.executeQuery();
+            if (rs.next()) {
+                ref = rs.getInt(1) + 1;
+            }
+            String sql = "insert into board values(num, ?, ?, ?, ?, now(), ?, ?, ?, 0, ?)";
+            pstmt = con.prepareStatement(sql);
+            pstmt.setString(1, bean.getWriter());
+            pstmt.setString(2, bean.getEmail());
+            pstmt.setString(3, bean.getSubject());
+            pstmt.setString(4, bean.getPassword());
+            pstmt.setInt(5, ref);
+            pstmt.setInt(6, re_step);
+            pstmt.setInt(7, re_level);
+            pstmt.setString(8, bean.getContent());
+            pstmt.executeUpdate();
+            con.close();
+        } catch (Exception e) {
+            e.printStackTrace();
+        }
+    }
+    public int getAllCount() {
+        getCon();
+        int count = 0;
+        try {
+            String sql = "select count(*) from board";
+            pstmt = con.prepareStatement(sql);
+            rs = pstmt.executeQuery(); // 값 저장한걸
+            if (rs.next()) { // 받아서
+                count = rs.getInt(1); // 카운트 변수에 넣자!
+            }
+            con.close();
+        } catch (Exception e) {
+            e.printStackTrace();
+        }
+        return count;
+    }
+    public BoardBean oneBoard(int num) {
+        // 조회수 증가, 번호를 기준으로 한 게시글에 대한 정보 가져오기
+        BoardBean bean = new BoardBean();
+        getCon();
+        try {
+            String readsql = "update board set readcount=readcount+1 where num=?";
+            pstmt = con.prepareStatement(readsql);
+            pstmt.setInt(1, num);
+            pstmt.executeUpdate(); // 절대 중요함!
+            String sql = "select * from board where num=?";
+            pstmt = con.prepareStatement(sql);
+            pstmt.setInt(1, num);
+            rs = pstmt.executeQuery();
+            if (rs.next()) {
+                bean.setNum(rs.getInt(1));
+                bean.setWriter(rs.getString(2));
+                bean.setEmail(rs.getString(3));
+                bean.setSubject(rs.getString(4));
+                bean.setPassword(rs.getString(5));
+                bean.setReg_date(rs.getDate(6).toString());
+                bean.setRef(rs.getInt(7));
+                bean.setRe_step(rs.getInt(8));
+                bean.setRe_level(rs.getInt(9));
+                bean.setReadcount(rs.getInt(10));
+                bean.setContent(rs.getString(11));
+            }
+            con.close();
+        } catch (Exception e) {
+            e.printStackTrace();
+        }
+        return bean;
+    }
+    public BoardBean oneUpdateBoard(int num) {
+        BoardBean bean = new BoardBean();
+        getCon();
+        try {
+            String sql = "select * from board where num=?";
+            pstmt = con.prepareStatement(sql);
+            pstmt.setInt(1, num);
+            rs = pstmt.executeQuery();
+            if (rs.next()) {
+                bean.setNum(rs.getInt(1));
+                bean.setWriter(rs.getString(2));
+                bean.setEmail(rs.getString(3));
+                bean.setSubject(rs.getString(4));
+                bean.setPassword(rs.getString(5));
+                bean.setReg_date(rs.getDate(6).toString());
+                bean.setRef(rs.getInt(7));
+                bean.setRe_step(rs.getInt(8));
+                bean.setRe_level(rs.getInt(9));
+                bean.setReadcount(rs.getInt(10));
+                bean.setContent(rs.getString(11));
+            }
+            con.close();
+        } catch (Exception e) {
+            e.printStackTrace();
+        }
+        return bean;
+    }
+    public String getPass(int num){ //UpdateProc의 ID(hidden) 받아옴
+        String pass = "";
+        try{
+            getCon();
+            String sql="select pass1 from member where id=?";
+            pstmt=con.prepareStatement(sql);
+            pstmt.setInt(1, num);
+            rs= pstmt.executeQuery();
+            if(rs.next()){
+                pass=rs.getString(1);
+            }
+            con.close();
+        } catch (Exception e) {
+            e.printStackTrace();
+        }
+        return pass;
+    }
+    public void updateBoard(BoardBean bean) {
+        getCon();
+        try{
+            String sql ="update board set subject=?, content=? where num=?";
+            pstmt=con.prepareStatement(sql);
+            pstmt.setString(1, bean.getSubject());
+            pstmt.setString(2, bean.getContent());
+            pstmt.setInt(3, bean.getNum());
+            pstmt.executeUpdate();
+        } catch (Exception e) {
+            e.printStackTrace();
+        }
+    }
+    public Vector&lt;BoardBean&gt; allBoard(int startRow, int endRow){
+        Vector&lt;BoardBean&gt; v = new Vector&lt;BoardBean&gt;();
+        getCon();
+        try {
+            String sql="select *from board order by ref desc, re_step asc limit ?,?";
+            pstmt=con.prepareStatement(sql);
+            pstmt.setInt(1, startRow-1);
+            pstmt.setInt(2, endRow);
+            rs=pstmt.executeQuery();
+            while(rs.next()){
+                BoardBean bean=new BoardBean();
+                bean.setNum(rs.getInt(1));
+                bean.setWriter(rs.getString(2));
+                bean.setEmail(rs.getString(3));
+                bean.setSubject(rs.getString(4));
+                bean.setPassword(rs.getString(5));
+                bean.setReg_date(rs.getDate(6).toString());
+                bean.setRef(rs.getInt(7));
+                bean.setRe_step(rs.getInt(8));
+                bean.setRe_level(rs.getInt(9));
+                bean.setReadcount(rs.getInt(10));
+                bean.setContent(rs.getString(11));
+                v.add(bean);
+            }
+            con.close();
+        }catch (Exception e) {
+            e.printStackTrace();
+        }
+        return v;
+    }
+}
+package kr.co.bit;
+public class BoardBean {
+    private int num;
+    private String writer;
+    private String email;
+    private String subject;
+    private String password;
+    private String reg_date;
+    private int ref;
+    private int re_step;
+    private int re_level;
+    private int readcount;
+    private String content;
+    public int getNum() {
+        return num;
+    }
+    public void setNum(int num) {
+        this.num = num;
+    }
+    public String getWriter() {
+        return writer;
+    }
+    public void setWriter(String writer) {
+        this.writer = writer;
+    }
+    public String getEmail() {
+        return email;
+    }
+    public void setEmail(String email) {
+        this.email = email;
+    }
+    public String getSubject() {
+        return subject;
+    }
+    public void setSubject(String subject) {
+        this.subject = subject;
+    }
+    public String getPassword() {
+        return password;
+    }
+    public void setPassword(String password) {
+        this.password = password;
+    }
+    public String getReg_date() {
+        return reg_date;
+    }
+    public void setReg_date(String reg_date) {
+        this.reg_date = reg_date;
+    }
+    public int getRef() {
+        return ref;
+    }
+    public void setRef(int ref) {
+        this.ref = ref;
+    }
+    public int getRe_step() {
+        return re_step;
+    }
+    public void setRe_step(int re_step) {
+        this.re_step = re_step;
+    }
+    public int getRe_level() {
+        return re_level;
+    }
+    public void setRe_level(int re_level) {
+        this.re_level = re_level;
+    }
+    public int getReadcount() {
+        return readcount;
+    }
+    public void setReadcount(int readcount) {
+        this.readcount = readcount;
+    }
+    public String getContent() {
+        return content;
+    }
+    public void setContent(String content) {
+        this.content = content;
+    }
+}
+</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6979,6 +7626,36 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFEEFFFF"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC3E88D"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFC792EA"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFFFCB6B"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -7020,7 +7697,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7068,6 +7745,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7386,8 +8066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50477DA0-4BC1-4335-9D01-289D71463095}">
   <dimension ref="A1:F326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1"/>
@@ -7735,7 +8415,7 @@
         <v>49</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1">
@@ -8102,10 +8782,10 @@
         <v>83</v>
       </c>
       <c r="D42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" customHeight="1">
@@ -8113,7 +8793,7 @@
         <v>45406</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
         <v>72</v>
@@ -8122,11 +8802,41 @@
         <v>100</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" customHeight="1"/>
-    <row r="45" spans="1:6" ht="30" customHeight="1"/>
+    <row r="44" spans="1:6" ht="30" customHeight="1">
+      <c r="A44" s="2">
+        <v>45407</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" customHeight="1">
+      <c r="A45" s="2">
+        <v>45407</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="16"/>
+    </row>
     <row r="46" spans="1:6" ht="30" customHeight="1"/>
     <row r="47" spans="1:6" ht="30" customHeight="1"/>
     <row r="48" spans="1:6" ht="30" customHeight="1"/>
@@ -8409,9 +9119,10 @@
     <row r="325" customFormat="1" ht="30" customHeight="1"/>
     <row r="326" customFormat="1" ht="30" customHeight="1"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E44:E45"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>